<commit_message>
CIFMM-2212 Creation of Event Summary profile
</commit_message>
<xml_diff>
--- a/output/EventSummary/composition-es-1.xlsx
+++ b/output/EventSummary/composition-es-1.xlsx
@@ -206,113 +206,113 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t>Composition.meta.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>xml:id (or equivalent in JSON)</t>
+  </si>
+  <si>
+    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Composition.meta.extension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Additional Content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>Composition.meta.versionId</t>
+  </si>
+  <si>
+    <t>Version specific identifier</t>
+  </si>
+  <si>
+    <t>The version specific identifier, as it appears in the version portion of the URL. This values changes when the resource is created, updated, or deleted.</t>
+  </si>
+  <si>
+    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
+  </si>
+  <si>
+    <t>Meta.versionId</t>
+  </si>
+  <si>
+    <t>Composition.meta.lastUpdated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instant {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>When the resource version last changed</t>
+  </si>
+  <si>
+    <t>When the resource last changed - e.g. when the version changed.</t>
+  </si>
+  <si>
+    <t>This value is always populated except when the resource is first being created. The server / resource manager sets this value; what a client provides is irrelevant.</t>
+  </si>
+  <si>
+    <t>Meta.lastUpdated</t>
+  </si>
+  <si>
+    <t>Composition.meta.profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uri {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Profiles this resource claims to conform to</t>
+  </si>
+  <si>
+    <t>A list of profiles (references to [StructureDefinition](structuredefinition.html#) resources) that this resource claims to conform to. The URL is a reference to [StructureDefinition.url]().</t>
+  </si>
+  <si>
+    <t>It is up to the server and/or other infrastructure of policy to determine whether/how these claims are verified and/or updated over time.  The list of profile URLs is a set.</t>
+  </si>
+  <si>
+    <t>Meta.profile</t>
+  </si>
+  <si>
     <t xml:space="preserve">inv-dh-cmp-01:One meta.profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-es-1' {Composition.meta.profile.where($this='http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-es-1').exists()}
 </t>
-  </si>
-  <si>
-    <t>Composition.meta.id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Composition.meta.extension</t>
-  </si>
-  <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Additional Content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>Composition.meta.versionId</t>
-  </si>
-  <si>
-    <t>Version specific identifier</t>
-  </si>
-  <si>
-    <t>The version specific identifier, as it appears in the version portion of the URL. This values changes when the resource is created, updated, or deleted.</t>
-  </si>
-  <si>
-    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
-  </si>
-  <si>
-    <t>Meta.versionId</t>
-  </si>
-  <si>
-    <t>Composition.meta.lastUpdated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">instant {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>When the resource version last changed</t>
-  </si>
-  <si>
-    <t>When the resource last changed - e.g. when the version changed.</t>
-  </si>
-  <si>
-    <t>This value is always populated except when the resource is first being created. The server / resource manager sets this value; what a client provides is irrelevant.</t>
-  </si>
-  <si>
-    <t>Meta.lastUpdated</t>
-  </si>
-  <si>
-    <t>Composition.meta.profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uri {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Profiles this resource claims to conform to</t>
-  </si>
-  <si>
-    <t>A list of profiles (references to [StructureDefinition](structuredefinition.html#) resources) that this resource claims to conform to. The URL is a reference to [StructureDefinition.url]().</t>
-  </si>
-  <si>
-    <t>It is up to the server and/or other infrastructure of policy to determine whether/how these claims are verified and/or updated over time.  The list of profile URLs is a set.</t>
-  </si>
-  <si>
-    <t>Meta.profile</t>
   </si>
   <si>
     <t>Composition.meta.security</t>
@@ -1421,7 +1421,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">inv-dh-cmp-03:A list of medication changes from this event or an assertion that there are no current medications shall be present, but not both {Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').exists() implies (Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is MedicationStatement).exists() xor Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is Observation ).exists())}
+    <t xml:space="preserve">inv-dh-cmp-03:A list of medication changes from this event or an assertion that there are no current medications shall be present, but not both {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '10160-0').exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '10160-0').entry.resolve().where($this is List).exists() xor Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '10160-0').entry.resolve().where($this is Observation ).exists())}
 </t>
   </si>
   <si>
@@ -1456,8 +1456,8 @@
     <t>Medical history</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-dh-cmp-04:At least one condition or procedure shall be present, or an assertion that there is no history shall be present, but not both {Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is value and value.coding.code = '1224831000168103').exists())}
-</t>
+    <t>inv-dh-cmp-04:At least one condition or procedure shall be present, or an assertion that there is no history shall be present, but not both {Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is value and value.coding.code = '1224831000168103').exists())}
+inv-dh-cmp-12:This section shall contain at most one assertion of no relevant finding entry and it shall assert no relevant medical history {Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is value and value.coding.code = '1224831000168103').exists())}</t>
   </si>
   <si>
     <t>immunisations</t>
@@ -1491,8 +1491,8 @@
     <t>Administered and/or non-administered vaccines</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-dh-cmp-05:At least one statement of vaccine or an assertion that there is no history of immunisation shall be present, but not both {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Immunization).exists() xor Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation ).exists())}
-</t>
+    <t>inv-dh-cmp-05:At least one statement of vaccine or an assertion that there is no history of immunisation shall be present, but not both {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Immunization).exists() xor Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation ).exists())}
+inv-dh-cmp-11:This section shall contain at most one assertion of no relevant finding entry and it shall assert no previous immunisations {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is value and value.coding.code = '1234401000168109').exists())}</t>
   </si>
 </sst>
 </file>
@@ -2116,7 +2116,7 @@
         <v>39</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>39</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -2153,13 +2153,13 @@
         <v>39</v>
       </c>
       <c r="J5" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K5" t="s" s="2">
+      <c r="L5" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L5" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -2210,22 +2210,22 @@
         <v>39</v>
       </c>
       <c r="AE5" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF5" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG5" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH5" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI5" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ5" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG5" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH5" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI5" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ5" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK5" t="s" s="2">
         <v>39</v>
@@ -2236,11 +2236,11 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
@@ -2259,16 +2259,16 @@
         <v>39</v>
       </c>
       <c r="J6" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K6" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="K6" t="s" s="2">
+      <c r="L6" t="s" s="2">
         <v>72</v>
       </c>
-      <c r="L6" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>73</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>74</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -2306,19 +2306,19 @@
         <v>39</v>
       </c>
       <c r="AA6" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB6" t="s" s="2">
         <v>75</v>
       </c>
-      <c r="AB6" t="s" s="2">
+      <c r="AC6" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD6" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="AC6" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD6" t="s" s="2">
+      <c r="AE6" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>40</v>
@@ -2333,7 +2333,7 @@
         <v>39</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK6" t="s" s="2">
         <v>39</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
@@ -2370,13 +2370,13 @@
         <v>52</v>
       </c>
       <c r="K7" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="L7" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="L7" t="s" s="2">
+      <c r="M7" t="s" s="2">
         <v>81</v>
-      </c>
-      <c r="M7" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -2426,7 +2426,7 @@
         <v>39</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>40</v>
@@ -2452,7 +2452,7 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -2475,16 +2475,16 @@
         <v>51</v>
       </c>
       <c r="J8" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="K8" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="K8" t="s" s="2">
+      <c r="L8" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="L8" t="s" s="2">
+      <c r="M8" t="s" s="2">
         <v>87</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>88</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2534,7 +2534,7 @@
         <v>39</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>40</v>
@@ -2560,7 +2560,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2583,16 +2583,16 @@
         <v>51</v>
       </c>
       <c r="J9" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="M9" t="s" s="2">
         <v>93</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>94</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2642,7 +2642,7 @@
         <v>39</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>40</v>
@@ -2654,7 +2654,7 @@
         <v>39</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>39</v>
@@ -2907,7 +2907,7 @@
         <v>51</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K12" t="s" s="2">
         <v>114</v>
@@ -3339,7 +3339,7 @@
         <v>39</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K16" t="s" s="2">
         <v>145</v>
@@ -3384,14 +3384,14 @@
         <v>39</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB16" s="2"/>
       <c r="AC16" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD16" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE16" t="s" s="2">
         <v>147</v>
@@ -3640,7 +3640,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3659,7 +3659,7 @@
         <v>39</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K19" t="s" s="2">
         <v>160</v>
@@ -3668,7 +3668,7 @@
         <v>161</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3954,7 +3954,7 @@
         <v>179</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>180</v>
@@ -4174,7 +4174,7 @@
         <v>201</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>193</v>
@@ -4641,7 +4641,7 @@
         <v>51</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K28" t="s" s="2">
         <v>237</v>
@@ -4913,7 +4913,7 @@
         <v>39</v>
       </c>
       <c r="AD30" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE30" t="s" s="2">
         <v>249</v>
@@ -4965,13 +4965,13 @@
         <v>39</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5022,22 +5022,22 @@
         <v>39</v>
       </c>
       <c r="AE31" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG31" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH31" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI31" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF31" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG31" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH31" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI31" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>39</v>
@@ -5071,7 +5071,7 @@
         <v>39</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K32" t="s" s="2">
         <v>145</v>
@@ -5116,17 +5116,17 @@
         <v>39</v>
       </c>
       <c r="AA32" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB32" s="2"/>
       <c r="AC32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD32" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE32" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AE32" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>40</v>
@@ -5234,7 +5234,7 @@
         <v>39</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -5283,7 +5283,7 @@
         <v>51</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K34" t="s" s="2">
         <v>160</v>
@@ -5292,7 +5292,7 @@
         <v>267</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -5829,13 +5829,13 @@
         <v>39</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5886,22 +5886,22 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG39" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH39" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI39" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG39" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>39</v>
@@ -5935,7 +5935,7 @@
         <v>39</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K40" t="s" s="2">
         <v>145</v>
@@ -5980,17 +5980,17 @@
         <v>39</v>
       </c>
       <c r="AA40" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB40" s="2"/>
       <c r="AC40" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD40" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE40" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -6098,7 +6098,7 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -6147,7 +6147,7 @@
         <v>51</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K42" t="s" s="2">
         <v>160</v>
@@ -6156,7 +6156,7 @@
         <v>267</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6799,13 +6799,13 @@
         <v>39</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K48" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K48" t="s" s="2">
+      <c r="L48" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6856,22 +6856,22 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG48" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH48" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI48" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ48" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>39</v>
@@ -6886,7 +6886,7 @@
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -6905,16 +6905,16 @@
         <v>39</v>
       </c>
       <c r="J49" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K49" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="K49" t="s" s="2">
+      <c r="L49" t="s" s="2">
         <v>72</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>73</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>74</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -6964,7 +6964,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6979,7 +6979,7 @@
         <v>39</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>39</v>
@@ -7013,7 +7013,7 @@
         <v>51</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K50" t="s" s="2">
         <v>160</v>
@@ -7022,7 +7022,7 @@
         <v>267</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -7445,13 +7445,13 @@
         <v>39</v>
       </c>
       <c r="J54" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K54" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K54" t="s" s="2">
+      <c r="L54" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7502,22 +7502,22 @@
         <v>39</v>
       </c>
       <c r="AE54" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK54" t="s" s="2">
         <v>39</v>
@@ -7532,7 +7532,7 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7551,16 +7551,16 @@
         <v>39</v>
       </c>
       <c r="J55" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K55" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="K55" t="s" s="2">
+      <c r="L55" t="s" s="2">
         <v>72</v>
       </c>
-      <c r="L55" t="s" s="2">
+      <c r="M55" t="s" s="2">
         <v>73</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>74</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -7610,7 +7610,7 @@
         <v>39</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>40</v>
@@ -7625,7 +7625,7 @@
         <v>39</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>39</v>
@@ -7659,7 +7659,7 @@
         <v>51</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K56" t="s" s="2">
         <v>160</v>
@@ -7668,7 +7668,7 @@
         <v>267</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
@@ -8056,7 +8056,7 @@
         <v>351</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>39</v>
@@ -8139,7 +8139,7 @@
         <v>39</v>
       </c>
       <c r="AD60" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE60" t="s" s="2">
         <v>352</v>
@@ -8191,13 +8191,13 @@
         <v>39</v>
       </c>
       <c r="J61" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K61" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K61" t="s" s="2">
+      <c r="L61" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8248,22 +8248,22 @@
         <v>39</v>
       </c>
       <c r="AE61" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF61" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG61" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>39</v>
@@ -8297,7 +8297,7 @@
         <v>39</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K62" t="s" s="2">
         <v>145</v>
@@ -8342,17 +8342,17 @@
         <v>39</v>
       </c>
       <c r="AA62" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB62" s="2"/>
       <c r="AC62" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE62" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8460,7 +8460,7 @@
         <v>39</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8509,7 +8509,7 @@
         <v>51</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K64" t="s" s="2">
         <v>160</v>
@@ -8518,7 +8518,7 @@
         <v>267</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8617,7 +8617,7 @@
         <v>39</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K65" t="s" s="2">
         <v>368</v>
@@ -9024,7 +9024,7 @@
         <v>392</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>193</v>
@@ -9134,7 +9134,7 @@
         <v>400</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>39</v>
@@ -9352,7 +9352,7 @@
         <v>415</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>39</v>
@@ -9599,13 +9599,13 @@
         <v>39</v>
       </c>
       <c r="J74" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K74" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K74" t="s" s="2">
+      <c r="L74" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -9656,22 +9656,22 @@
         <v>39</v>
       </c>
       <c r="AE74" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF74" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG74" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH74" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI74" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ74" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK74" t="s" s="2">
         <v>39</v>
@@ -9705,7 +9705,7 @@
         <v>39</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K75" t="s" s="2">
         <v>145</v>
@@ -9750,17 +9750,17 @@
         <v>39</v>
       </c>
       <c r="AA75" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB75" s="2"/>
       <c r="AC75" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE75" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AE75" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>40</v>
@@ -9868,7 +9868,7 @@
         <v>39</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>40</v>
@@ -9917,7 +9917,7 @@
         <v>51</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K77" t="s" s="2">
         <v>160</v>
@@ -9926,7 +9926,7 @@
         <v>267</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
@@ -10025,7 +10025,7 @@
         <v>39</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K78" t="s" s="2">
         <v>368</v>
@@ -10432,7 +10432,7 @@
         <v>392</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL81" t="s" s="2">
         <v>193</v>
@@ -10542,7 +10542,7 @@
         <v>400</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL82" t="s" s="2">
         <v>39</v>
@@ -10760,7 +10760,7 @@
         <v>415</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL84" t="s" s="2">
         <v>39</v>
@@ -11007,13 +11007,13 @@
         <v>39</v>
       </c>
       <c r="J87" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K87" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K87" t="s" s="2">
+      <c r="L87" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L87" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -11064,22 +11064,22 @@
         <v>39</v>
       </c>
       <c r="AE87" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG87" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ87" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF87" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG87" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH87" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI87" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ87" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK87" t="s" s="2">
         <v>39</v>
@@ -11113,7 +11113,7 @@
         <v>39</v>
       </c>
       <c r="J88" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K88" t="s" s="2">
         <v>145</v>
@@ -11158,17 +11158,17 @@
         <v>39</v>
       </c>
       <c r="AA88" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB88" s="2"/>
       <c r="AC88" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD88" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE88" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AE88" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>40</v>
@@ -11276,7 +11276,7 @@
         <v>39</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>40</v>
@@ -11325,7 +11325,7 @@
         <v>51</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K90" t="s" s="2">
         <v>160</v>
@@ -11334,7 +11334,7 @@
         <v>267</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N90" s="2"/>
       <c r="O90" t="s" s="2">
@@ -11433,7 +11433,7 @@
         <v>39</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K91" t="s" s="2">
         <v>368</v>
@@ -11840,7 +11840,7 @@
         <v>392</v>
       </c>
       <c r="AK94" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL94" t="s" s="2">
         <v>193</v>
@@ -11950,7 +11950,7 @@
         <v>400</v>
       </c>
       <c r="AK95" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL95" t="s" s="2">
         <v>39</v>
@@ -12166,7 +12166,7 @@
         <v>415</v>
       </c>
       <c r="AK97" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL97" t="s" s="2">
         <v>39</v>
@@ -12413,13 +12413,13 @@
         <v>39</v>
       </c>
       <c r="J100" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K100" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K100" t="s" s="2">
+      <c r="L100" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L100" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
@@ -12470,22 +12470,22 @@
         <v>39</v>
       </c>
       <c r="AE100" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG100" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ100" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF100" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG100" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH100" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI100" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ100" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK100" t="s" s="2">
         <v>39</v>
@@ -12519,7 +12519,7 @@
         <v>39</v>
       </c>
       <c r="J101" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K101" t="s" s="2">
         <v>145</v>
@@ -12564,17 +12564,17 @@
         <v>39</v>
       </c>
       <c r="AA101" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB101" s="2"/>
       <c r="AC101" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD101" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE101" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AE101" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>40</v>
@@ -12682,7 +12682,7 @@
         <v>39</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>40</v>
@@ -12731,7 +12731,7 @@
         <v>51</v>
       </c>
       <c r="J103" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K103" t="s" s="2">
         <v>160</v>
@@ -12740,7 +12740,7 @@
         <v>267</v>
       </c>
       <c r="M103" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N103" s="2"/>
       <c r="O103" t="s" s="2">
@@ -12839,7 +12839,7 @@
         <v>39</v>
       </c>
       <c r="J104" t="s" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K104" t="s" s="2">
         <v>368</v>
@@ -13246,7 +13246,7 @@
         <v>392</v>
       </c>
       <c r="AK107" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL107" t="s" s="2">
         <v>193</v>
@@ -13356,7 +13356,7 @@
         <v>400</v>
       </c>
       <c r="AK108" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL108" t="s" s="2">
         <v>39</v>
@@ -13572,7 +13572,7 @@
         <v>415</v>
       </c>
       <c r="AK110" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL110" t="s" s="2">
         <v>39</v>
@@ -13819,13 +13819,13 @@
         <v>39</v>
       </c>
       <c r="J113" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K113" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K113" t="s" s="2">
+      <c r="L113" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L113" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
@@ -13876,22 +13876,22 @@
         <v>39</v>
       </c>
       <c r="AE113" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF113" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG113" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH113" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI113" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ113" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF113" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG113" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH113" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI113" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ113" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK113" t="s" s="2">
         <v>39</v>
@@ -13925,7 +13925,7 @@
         <v>39</v>
       </c>
       <c r="J114" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K114" t="s" s="2">
         <v>145</v>
@@ -13970,17 +13970,17 @@
         <v>39</v>
       </c>
       <c r="AA114" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB114" s="2"/>
       <c r="AC114" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD114" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE114" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AE114" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>40</v>
@@ -14088,7 +14088,7 @@
         <v>39</v>
       </c>
       <c r="AE115" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF115" t="s" s="2">
         <v>40</v>
@@ -14137,7 +14137,7 @@
         <v>51</v>
       </c>
       <c r="J116" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K116" t="s" s="2">
         <v>160</v>
@@ -14146,7 +14146,7 @@
         <v>267</v>
       </c>
       <c r="M116" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N116" s="2"/>
       <c r="O116" t="s" s="2">
@@ -14245,7 +14245,7 @@
         <v>39</v>
       </c>
       <c r="J117" t="s" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K117" t="s" s="2">
         <v>368</v>
@@ -14652,7 +14652,7 @@
         <v>392</v>
       </c>
       <c r="AK120" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL120" t="s" s="2">
         <v>193</v>
@@ -14762,7 +14762,7 @@
         <v>400</v>
       </c>
       <c r="AK121" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL121" t="s" s="2">
         <v>39</v>
@@ -14978,7 +14978,7 @@
         <v>415</v>
       </c>
       <c r="AK123" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL123" t="s" s="2">
         <v>39</v>
@@ -15225,13 +15225,13 @@
         <v>39</v>
       </c>
       <c r="J126" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K126" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="K126" t="s" s="2">
+      <c r="L126" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="L126" t="s" s="2">
-        <v>66</v>
       </c>
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
@@ -15282,22 +15282,22 @@
         <v>39</v>
       </c>
       <c r="AE126" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="AF126" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG126" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH126" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI126" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ126" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="AF126" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG126" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH126" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI126" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ126" t="s" s="2">
-        <v>68</v>
       </c>
       <c r="AK126" t="s" s="2">
         <v>39</v>
@@ -15331,7 +15331,7 @@
         <v>39</v>
       </c>
       <c r="J127" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K127" t="s" s="2">
         <v>145</v>
@@ -15376,17 +15376,17 @@
         <v>39</v>
       </c>
       <c r="AA127" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB127" s="2"/>
       <c r="AC127" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD127" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE127" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="AE127" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AF127" t="s" s="2">
         <v>40</v>
@@ -15494,7 +15494,7 @@
         <v>39</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AF128" t="s" s="2">
         <v>40</v>
@@ -15543,7 +15543,7 @@
         <v>51</v>
       </c>
       <c r="J129" t="s" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K129" t="s" s="2">
         <v>160</v>
@@ -15552,7 +15552,7 @@
         <v>267</v>
       </c>
       <c r="M129" t="s" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N129" s="2"/>
       <c r="O129" t="s" s="2">
@@ -15651,7 +15651,7 @@
         <v>39</v>
       </c>
       <c r="J130" t="s" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K130" t="s" s="2">
         <v>368</v>
@@ -16058,7 +16058,7 @@
         <v>392</v>
       </c>
       <c r="AK133" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL133" t="s" s="2">
         <v>193</v>
@@ -16168,7 +16168,7 @@
         <v>400</v>
       </c>
       <c r="AK134" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL134" t="s" s="2">
         <v>39</v>
@@ -16384,7 +16384,7 @@
         <v>415</v>
       </c>
       <c r="AK136" t="s" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL136" t="s" s="2">
         <v>39</v>

</xml_diff>

<commit_message>
CIFMM-2212 changes after 1st peer review
</commit_message>
<xml_diff>
--- a/output/EventSummary/composition-es-1.xlsx
+++ b/output/EventSummary/composition-es-1.xlsx
@@ -206,6 +206,10 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t xml:space="preserve">inv-dh-cmp-01:One meta.profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-es-1' {Composition.meta.profile.where($this='http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-es-1').exists()}
+</t>
+  </si>
+  <si>
     <t>Composition.meta.id</t>
   </si>
   <si>
@@ -302,17 +306,13 @@
     <t>Profiles this resource claims to conform to</t>
   </si>
   <si>
-    <t>A list of profiles (references to [StructureDefinition](https://build.fhir.org/ig/hl7au/au-fhir-base/structuredefinition.html#) resources) that this resource claims to conform to. The URL is a reference to [StructureDefinition.url](https://build.fhir.org/ig/hl7au/au-fhir-base/).</t>
+    <t>A list of profiles (references to [StructureDefinition](structuredefinition.html#) resources) that this resource claims to conform to. The URL is a reference to [StructureDefinition.url]().</t>
   </si>
   <si>
     <t>It is up to the server and/or other infrastructure of policy to determine whether/how these claims are verified and/or updated over time.  The list of profile URLs is a set.</t>
   </si>
   <si>
     <t>Meta.profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inv-dh-cmp-01:One meta.profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-es-1' {Composition.meta.profile.where($this='http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-es-1').exists()}
-</t>
   </si>
   <si>
     <t>Composition.meta.security</t>
@@ -2116,7 +2116,7 @@
         <v>39</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>39</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -2153,13 +2153,13 @@
         <v>39</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -2210,7 +2210,7 @@
         <v>39</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>40</v>
@@ -2225,7 +2225,7 @@
         <v>39</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK5" t="s" s="2">
         <v>39</v>
@@ -2236,11 +2236,11 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
@@ -2259,16 +2259,16 @@
         <v>39</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -2306,19 +2306,19 @@
         <v>39</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AC6" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>40</v>
@@ -2333,7 +2333,7 @@
         <v>39</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK6" t="s" s="2">
         <v>39</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
@@ -2370,13 +2370,13 @@
         <v>52</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -2426,7 +2426,7 @@
         <v>39</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>40</v>
@@ -2452,7 +2452,7 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -2475,16 +2475,16 @@
         <v>51</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2534,7 +2534,7 @@
         <v>39</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>40</v>
@@ -2560,7 +2560,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2583,16 +2583,16 @@
         <v>51</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2642,7 +2642,7 @@
         <v>39</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>40</v>
@@ -2654,7 +2654,7 @@
         <v>39</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>39</v>
@@ -2907,7 +2907,7 @@
         <v>51</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K12" t="s" s="2">
         <v>114</v>
@@ -3339,7 +3339,7 @@
         <v>39</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K16" t="s" s="2">
         <v>145</v>
@@ -3384,14 +3384,14 @@
         <v>39</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB16" s="2"/>
       <c r="AC16" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD16" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE16" t="s" s="2">
         <v>147</v>
@@ -3640,7 +3640,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3659,7 +3659,7 @@
         <v>39</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K19" t="s" s="2">
         <v>160</v>
@@ -3668,7 +3668,7 @@
         <v>161</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3954,7 +3954,7 @@
         <v>179</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>180</v>
@@ -4174,7 +4174,7 @@
         <v>201</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>193</v>
@@ -4641,7 +4641,7 @@
         <v>51</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K28" t="s" s="2">
         <v>237</v>
@@ -4913,7 +4913,7 @@
         <v>39</v>
       </c>
       <c r="AD30" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE30" t="s" s="2">
         <v>249</v>
@@ -4965,13 +4965,13 @@
         <v>39</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5022,7 +5022,7 @@
         <v>39</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>40</v>
@@ -5037,7 +5037,7 @@
         <v>39</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>39</v>
@@ -5071,7 +5071,7 @@
         <v>39</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K32" t="s" s="2">
         <v>145</v>
@@ -5116,17 +5116,17 @@
         <v>39</v>
       </c>
       <c r="AA32" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB32" s="2"/>
       <c r="AC32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD32" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>40</v>
@@ -5234,7 +5234,7 @@
         <v>39</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -5283,7 +5283,7 @@
         <v>51</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K34" t="s" s="2">
         <v>160</v>
@@ -5292,7 +5292,7 @@
         <v>267</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -5829,13 +5829,13 @@
         <v>39</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5886,7 +5886,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5901,7 +5901,7 @@
         <v>39</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>39</v>
@@ -5935,7 +5935,7 @@
         <v>39</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K40" t="s" s="2">
         <v>145</v>
@@ -5980,17 +5980,17 @@
         <v>39</v>
       </c>
       <c r="AA40" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB40" s="2"/>
       <c r="AC40" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD40" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -6098,7 +6098,7 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -6147,7 +6147,7 @@
         <v>51</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K42" t="s" s="2">
         <v>160</v>
@@ -6156,7 +6156,7 @@
         <v>267</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6799,13 +6799,13 @@
         <v>39</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6856,7 +6856,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6871,7 +6871,7 @@
         <v>39</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>39</v>
@@ -6886,7 +6886,7 @@
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -6905,16 +6905,16 @@
         <v>39</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -6964,7 +6964,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6979,7 +6979,7 @@
         <v>39</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>39</v>
@@ -7013,7 +7013,7 @@
         <v>51</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K50" t="s" s="2">
         <v>160</v>
@@ -7022,7 +7022,7 @@
         <v>267</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -7445,13 +7445,13 @@
         <v>39</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7502,7 +7502,7 @@
         <v>39</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>40</v>
@@ -7517,7 +7517,7 @@
         <v>39</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK54" t="s" s="2">
         <v>39</v>
@@ -7532,7 +7532,7 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7551,16 +7551,16 @@
         <v>39</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -7610,7 +7610,7 @@
         <v>39</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>40</v>
@@ -7625,7 +7625,7 @@
         <v>39</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>39</v>
@@ -7659,7 +7659,7 @@
         <v>51</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K56" t="s" s="2">
         <v>160</v>
@@ -7668,7 +7668,7 @@
         <v>267</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
@@ -8056,7 +8056,7 @@
         <v>351</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>39</v>
@@ -8139,7 +8139,7 @@
         <v>39</v>
       </c>
       <c r="AD60" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE60" t="s" s="2">
         <v>352</v>
@@ -8191,13 +8191,13 @@
         <v>39</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8248,7 +8248,7 @@
         <v>39</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>40</v>
@@ -8263,7 +8263,7 @@
         <v>39</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>39</v>
@@ -8297,7 +8297,7 @@
         <v>39</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K62" t="s" s="2">
         <v>145</v>
@@ -8342,17 +8342,17 @@
         <v>39</v>
       </c>
       <c r="AA62" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB62" s="2"/>
       <c r="AC62" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD62" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8460,7 +8460,7 @@
         <v>39</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8509,7 +8509,7 @@
         <v>51</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K64" t="s" s="2">
         <v>160</v>
@@ -8518,7 +8518,7 @@
         <v>267</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8617,7 +8617,7 @@
         <v>39</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K65" t="s" s="2">
         <v>368</v>
@@ -9024,7 +9024,7 @@
         <v>392</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>193</v>
@@ -9134,7 +9134,7 @@
         <v>400</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>39</v>
@@ -9352,7 +9352,7 @@
         <v>415</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>39</v>
@@ -9599,13 +9599,13 @@
         <v>39</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -9656,7 +9656,7 @@
         <v>39</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>40</v>
@@ -9671,7 +9671,7 @@
         <v>39</v>
       </c>
       <c r="AJ74" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK74" t="s" s="2">
         <v>39</v>
@@ -9705,7 +9705,7 @@
         <v>39</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K75" t="s" s="2">
         <v>145</v>
@@ -9750,17 +9750,17 @@
         <v>39</v>
       </c>
       <c r="AA75" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB75" s="2"/>
       <c r="AC75" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD75" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>40</v>
@@ -9868,7 +9868,7 @@
         <v>39</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>40</v>
@@ -9917,7 +9917,7 @@
         <v>51</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K77" t="s" s="2">
         <v>160</v>
@@ -9926,7 +9926,7 @@
         <v>267</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
@@ -10025,7 +10025,7 @@
         <v>39</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K78" t="s" s="2">
         <v>368</v>
@@ -10432,7 +10432,7 @@
         <v>392</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL81" t="s" s="2">
         <v>193</v>
@@ -10542,7 +10542,7 @@
         <v>400</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL82" t="s" s="2">
         <v>39</v>
@@ -10760,7 +10760,7 @@
         <v>415</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL84" t="s" s="2">
         <v>39</v>
@@ -11007,13 +11007,13 @@
         <v>39</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -11064,7 +11064,7 @@
         <v>39</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>40</v>
@@ -11079,7 +11079,7 @@
         <v>39</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK87" t="s" s="2">
         <v>39</v>
@@ -11113,7 +11113,7 @@
         <v>39</v>
       </c>
       <c r="J88" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K88" t="s" s="2">
         <v>145</v>
@@ -11158,17 +11158,17 @@
         <v>39</v>
       </c>
       <c r="AA88" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB88" s="2"/>
       <c r="AC88" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD88" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>40</v>
@@ -11276,7 +11276,7 @@
         <v>39</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>40</v>
@@ -11325,7 +11325,7 @@
         <v>51</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K90" t="s" s="2">
         <v>160</v>
@@ -11334,7 +11334,7 @@
         <v>267</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N90" s="2"/>
       <c r="O90" t="s" s="2">
@@ -11433,7 +11433,7 @@
         <v>39</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K91" t="s" s="2">
         <v>368</v>
@@ -11840,7 +11840,7 @@
         <v>392</v>
       </c>
       <c r="AK94" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL94" t="s" s="2">
         <v>193</v>
@@ -11950,7 +11950,7 @@
         <v>400</v>
       </c>
       <c r="AK95" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL95" t="s" s="2">
         <v>39</v>
@@ -12166,7 +12166,7 @@
         <v>415</v>
       </c>
       <c r="AK97" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL97" t="s" s="2">
         <v>39</v>
@@ -12413,13 +12413,13 @@
         <v>39</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
@@ -12470,7 +12470,7 @@
         <v>39</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>40</v>
@@ -12485,7 +12485,7 @@
         <v>39</v>
       </c>
       <c r="AJ100" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK100" t="s" s="2">
         <v>39</v>
@@ -12519,7 +12519,7 @@
         <v>39</v>
       </c>
       <c r="J101" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K101" t="s" s="2">
         <v>145</v>
@@ -12564,17 +12564,17 @@
         <v>39</v>
       </c>
       <c r="AA101" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB101" s="2"/>
       <c r="AC101" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD101" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>40</v>
@@ -12682,7 +12682,7 @@
         <v>39</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>40</v>
@@ -12731,7 +12731,7 @@
         <v>51</v>
       </c>
       <c r="J103" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K103" t="s" s="2">
         <v>160</v>
@@ -12740,7 +12740,7 @@
         <v>267</v>
       </c>
       <c r="M103" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N103" s="2"/>
       <c r="O103" t="s" s="2">
@@ -12839,7 +12839,7 @@
         <v>39</v>
       </c>
       <c r="J104" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K104" t="s" s="2">
         <v>368</v>
@@ -13246,7 +13246,7 @@
         <v>392</v>
       </c>
       <c r="AK107" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL107" t="s" s="2">
         <v>193</v>
@@ -13356,7 +13356,7 @@
         <v>400</v>
       </c>
       <c r="AK108" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL108" t="s" s="2">
         <v>39</v>
@@ -13572,7 +13572,7 @@
         <v>415</v>
       </c>
       <c r="AK110" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL110" t="s" s="2">
         <v>39</v>
@@ -13819,13 +13819,13 @@
         <v>39</v>
       </c>
       <c r="J113" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
@@ -13876,7 +13876,7 @@
         <v>39</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>40</v>
@@ -13891,7 +13891,7 @@
         <v>39</v>
       </c>
       <c r="AJ113" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK113" t="s" s="2">
         <v>39</v>
@@ -13925,7 +13925,7 @@
         <v>39</v>
       </c>
       <c r="J114" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K114" t="s" s="2">
         <v>145</v>
@@ -13970,17 +13970,17 @@
         <v>39</v>
       </c>
       <c r="AA114" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB114" s="2"/>
       <c r="AC114" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD114" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>40</v>
@@ -14088,7 +14088,7 @@
         <v>39</v>
       </c>
       <c r="AE115" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF115" t="s" s="2">
         <v>40</v>
@@ -14137,7 +14137,7 @@
         <v>51</v>
       </c>
       <c r="J116" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K116" t="s" s="2">
         <v>160</v>
@@ -14146,7 +14146,7 @@
         <v>267</v>
       </c>
       <c r="M116" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N116" s="2"/>
       <c r="O116" t="s" s="2">
@@ -14245,7 +14245,7 @@
         <v>39</v>
       </c>
       <c r="J117" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K117" t="s" s="2">
         <v>368</v>
@@ -14652,7 +14652,7 @@
         <v>392</v>
       </c>
       <c r="AK120" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL120" t="s" s="2">
         <v>193</v>
@@ -14762,7 +14762,7 @@
         <v>400</v>
       </c>
       <c r="AK121" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL121" t="s" s="2">
         <v>39</v>
@@ -14978,7 +14978,7 @@
         <v>415</v>
       </c>
       <c r="AK123" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL123" t="s" s="2">
         <v>39</v>
@@ -15225,13 +15225,13 @@
         <v>39</v>
       </c>
       <c r="J126" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K126" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L126" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
@@ -15282,7 +15282,7 @@
         <v>39</v>
       </c>
       <c r="AE126" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF126" t="s" s="2">
         <v>40</v>
@@ -15297,7 +15297,7 @@
         <v>39</v>
       </c>
       <c r="AJ126" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AK126" t="s" s="2">
         <v>39</v>
@@ -15331,7 +15331,7 @@
         <v>39</v>
       </c>
       <c r="J127" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K127" t="s" s="2">
         <v>145</v>
@@ -15376,17 +15376,17 @@
         <v>39</v>
       </c>
       <c r="AA127" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB127" s="2"/>
       <c r="AC127" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD127" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE127" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF127" t="s" s="2">
         <v>40</v>
@@ -15494,7 +15494,7 @@
         <v>39</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF128" t="s" s="2">
         <v>40</v>
@@ -15543,7 +15543,7 @@
         <v>51</v>
       </c>
       <c r="J129" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K129" t="s" s="2">
         <v>160</v>
@@ -15552,7 +15552,7 @@
         <v>267</v>
       </c>
       <c r="M129" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N129" s="2"/>
       <c r="O129" t="s" s="2">
@@ -15651,7 +15651,7 @@
         <v>39</v>
       </c>
       <c r="J130" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K130" t="s" s="2">
         <v>368</v>
@@ -16058,7 +16058,7 @@
         <v>392</v>
       </c>
       <c r="AK133" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL133" t="s" s="2">
         <v>193</v>
@@ -16168,7 +16168,7 @@
         <v>400</v>
       </c>
       <c r="AK134" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL134" t="s" s="2">
         <v>39</v>
@@ -16384,7 +16384,7 @@
         <v>415</v>
       </c>
       <c r="AK136" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL136" t="s" s="2">
         <v>39</v>

</xml_diff>

<commit_message>
CIFMM-2212 Changes to 3 definition tags in resource: composition-es-1 as per peer review.
</commit_message>
<xml_diff>
--- a/output/EventSummary/composition-es-1.xlsx
+++ b/output/EventSummary/composition-es-1.xlsx
@@ -1339,7 +1339,7 @@
     <t>Event Overview</t>
   </si>
   <si>
-    <t>It is expected that section.text is populated from the Encounter Description element of the Encounter entry.</t>
+    <t>Summary information concerning the event.</t>
   </si>
   <si>
     <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Event Details"/&gt;</t>
@@ -1399,7 +1399,7 @@
     <t>Medications</t>
   </si>
   <si>
-    <t>Medicines that the patient is currently taking including self-prescribed, clinician prescribed and nonprescription medication.</t>
+    <t>Information about medicines that are relevant to the encounter. The medicines included do not constitute a full medications list, but are those medicines that have specifically changed as a result of the encounter, or those medicines directly relevant to the encounter.</t>
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
@@ -1466,7 +1466,7 @@
     <t>Immunisations</t>
   </si>
   <si>
-    <t>Information about the immunisation history, i.e. administered vaccines, of a patient.</t>
+    <t>Information about vaccinations administered or reported to be administered during this encounter. This may include statements that a patient has not had a particular vaccine administered.</t>
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}

</xml_diff>